<commit_message>
0.1.05 - Change algorithm for divide members
</commit_message>
<xml_diff>
--- a/Source/Excel/Test/Frame_01.xlsx
+++ b/Source/Excel/Test/Frame_01.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aleksei\Havings\Code\demo.local\Source\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aleksei\Havings\Code\demo.local\Source\Excel\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -524,7 +524,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
0.01.09 - Finish to change algorithm of load application
</commit_message>
<xml_diff>
--- a/Source/Excel/Test/Frame_01.xlsx
+++ b/Source/Excel/Test/Frame_01.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
   <si>
     <t>GOST 26020</t>
   </si>
@@ -521,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,57 +724,57 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="1">
+        <v>90</v>
+      </c>
+      <c r="I6" s="6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="1">
+        <v>5</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B7" s="11" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>5</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="6">
-        <v>1</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="1">
-        <v>5</v>
-      </c>
-      <c r="L7" s="1">
-        <v>0</v>
-      </c>
-      <c r="M7" s="1">
-        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -801,70 +801,70 @@
         <v>1</v>
       </c>
       <c r="J8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="1">
+        <v>5</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>5</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="6">
+        <v>1</v>
+      </c>
+      <c r="J9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K8" s="1">
-        <v>0</v>
-      </c>
-      <c r="L8" s="1">
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
         <v>3</v>
       </c>
-      <c r="M8" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="M9" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B10" s="11" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0</v>
-      </c>
-      <c r="I10" s="6">
-        <v>1</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K10" s="1">
-        <v>4.5</v>
-      </c>
-      <c r="L10" s="1">
-        <v>0</v>
-      </c>
-      <c r="M10" s="1">
-        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
@@ -873,7 +873,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>7</v>
@@ -894,12 +894,53 @@
         <v>8</v>
       </c>
       <c r="K11" s="1">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="L11" s="1">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="6">
+        <v>1</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
         <v>2.5</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M12" s="1">
         <v>5</v>
       </c>
     </row>

</xml_diff>